<commit_message>
Updated aquifer, surface elevation, etc... Week 9
</commit_message>
<xml_diff>
--- a/ModelsData/gab_soils_dev2.xlsx
+++ b/ModelsData/gab_soils_dev2.xlsx
@@ -9,11 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9465" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9465" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="gab_soils_dev2" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$B$242</definedName>
@@ -23,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="105">
   <si>
     <t>FID</t>
   </si>
@@ -153,6 +156,192 @@
   <si>
     <t>Psi</t>
   </si>
+  <si>
+    <t>soiltype</t>
+  </si>
+  <si>
+    <t>areaac</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>psi</t>
+  </si>
+  <si>
+    <t>phi</t>
+  </si>
+  <si>
+    <t>fc</t>
+  </si>
+  <si>
+    <t>wp</t>
+  </si>
+  <si>
+    <t>[JUNCTIONS]</t>
+  </si>
+  <si>
+    <t>;;Name</t>
+  </si>
+  <si>
+    <t>Elevation</t>
+  </si>
+  <si>
+    <t>MaxDepth</t>
+  </si>
+  <si>
+    <t>InitDepth</t>
+  </si>
+  <si>
+    <t>SurDepth</t>
+  </si>
+  <si>
+    <t>Aponded</t>
+  </si>
+  <si>
+    <t>;;--------------</t>
+  </si>
+  <si>
+    <t>----------</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>J5</t>
+  </si>
+  <si>
+    <t>J6</t>
+  </si>
+  <si>
+    <t>J7</t>
+  </si>
+  <si>
+    <t>J8</t>
+  </si>
+  <si>
+    <t>J9</t>
+  </si>
+  <si>
+    <t>J10</t>
+  </si>
+  <si>
+    <t>J11</t>
+  </si>
+  <si>
+    <t>J12</t>
+  </si>
+  <si>
+    <t>J13</t>
+  </si>
+  <si>
+    <t>J14</t>
+  </si>
+  <si>
+    <t>J15</t>
+  </si>
+  <si>
+    <t>J16</t>
+  </si>
+  <si>
+    <t>J17</t>
+  </si>
+  <si>
+    <t>J18</t>
+  </si>
+  <si>
+    <t>J19</t>
+  </si>
+  <si>
+    <t>J20</t>
+  </si>
+  <si>
+    <t>J21</t>
+  </si>
+  <si>
+    <t>J22</t>
+  </si>
+  <si>
+    <t>J23</t>
+  </si>
+  <si>
+    <t>J24</t>
+  </si>
+  <si>
+    <t>J25</t>
+  </si>
+  <si>
+    <t>J26</t>
+  </si>
+  <si>
+    <t>J27</t>
+  </si>
+  <si>
+    <t>J28</t>
+  </si>
+  <si>
+    <t>S7</t>
+  </si>
+  <si>
+    <t>S8</t>
+  </si>
+  <si>
+    <t>S9</t>
+  </si>
+  <si>
+    <t>S10</t>
+  </si>
+  <si>
+    <t>S11</t>
+  </si>
+  <si>
+    <t>S12</t>
+  </si>
+  <si>
+    <t>S13</t>
+  </si>
+  <si>
+    <t>S14</t>
+  </si>
+  <si>
+    <t>S15</t>
+  </si>
+  <si>
+    <t>S16</t>
+  </si>
+  <si>
+    <t>S17</t>
+  </si>
+  <si>
+    <t>S18</t>
+  </si>
+  <si>
+    <t>S19</t>
+  </si>
+  <si>
+    <t>S20</t>
+  </si>
+  <si>
+    <t>S21</t>
+  </si>
+  <si>
+    <t>S22</t>
+  </si>
+  <si>
+    <t>S23</t>
+  </si>
+  <si>
+    <t>S24</t>
+  </si>
 </sst>
 </file>
 
@@ -163,7 +352,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -294,6 +483,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -646,13 +842,17 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="18" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="18" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="18" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -15008,95 +15208,97 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="S23" sqref="S23"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="1" max="1" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="10.140625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <f>SUMIFS(gab_soils_dev2!$S$2:$S$237,gab_soils_dev2!$N$2:$N$237,Sheet1!A2,gab_soils_dev2!$R$2:$R$237,Sheet1!B2)</f>
         <v>2.7800333999999998</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>4.74</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <f>D2*C2</f>
         <v>13.177358315999999</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="2">
         <f>SUM(E2:E5)/SUM($C$2:$C$5)</f>
         <v>0.21360690123871606</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
         <f>D2*C2</f>
         <v>13.177358315999999</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="3">
         <f>SUM(G2:G5)/SUM(C2:C5)</f>
         <v>0.21360690123871606</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="1">
         <f>IF(D2=4.74,5,IF(D2=0.04,3,1))</f>
         <v>5</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="1">
         <f>I2*C2</f>
         <v>13.900167</v>
       </c>
-      <c r="K2" s="1">
+      <c r="K2" s="3">
         <f>SUM(J2:J5)/SUM($C$2:$C$5)</f>
         <v>1.1775720268118623</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="1">
         <v>1.93</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2" s="4">
         <f>L2*C2</f>
         <v>5.3654644619999994</v>
       </c>
@@ -15106,168 +15308,168 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <f>SUMIFS(gab_soils_dev2!$S$2:$S$237,gab_soils_dev2!$N$2:$N$237,Sheet1!A3,gab_soils_dev2!$R$2:$R$237,Sheet1!B3)</f>
         <v>61.6526985</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>0.01</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <f t="shared" ref="E3:E44" si="0">D3*C3</f>
         <v>0.61652698500000003</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
         <f t="shared" ref="G3:G44" si="1">D3*C3</f>
         <v>0.61652698500000003</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="1">
         <f t="shared" ref="I3:I44" si="2">IF(D3=4.74,5,IF(D3=0.04,3,1))</f>
         <v>1</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="1">
         <f t="shared" ref="J3:J44" si="3">I3*C3</f>
         <v>61.6526985</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="1">
         <v>12.6</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3" s="4">
         <f>L3*C3</f>
         <v>776.82400109999992</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <f>SUMIFS(gab_soils_dev2!$S$2:$S$237,gab_soils_dev2!$N$2:$N$237,Sheet1!A4,gab_soils_dev2!$R$2:$R$237,Sheet1!B4)</f>
         <v>0.14825750000000001</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>0.04</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <f t="shared" si="0"/>
         <v>5.9303000000000003E-3</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1">
         <f t="shared" si="1"/>
         <v>5.9303000000000003E-3</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="1">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="1">
         <f t="shared" si="3"/>
         <v>0.44477250000000002</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="1">
         <v>10.63</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4" s="4">
         <f>L4*C4</f>
         <v>1.5759772250000004</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <f>SUMIFS(gab_soils_dev2!$S$2:$S$237,gab_soils_dev2!$N$2:$N$237,Sheet1!A5,gab_soils_dev2!$R$2:$R$237,Sheet1!B5)</f>
         <v>2.8055199999999999E-2</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>0.04</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <f t="shared" si="0"/>
         <v>1.122208E-3</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
         <f t="shared" si="1"/>
         <v>1.122208E-3</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="1">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="1">
         <f t="shared" si="3"/>
         <v>8.4165599999999993E-2</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="1">
         <v>10.63</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5" s="4">
         <f>L5*C5</f>
         <v>0.29822677600000003</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="M6" s="2"/>
+      <c r="M6" s="4"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <f>SUMIFS(gab_soils_dev2!$S$2:$S$237,gab_soils_dev2!$N$2:$N$237,Sheet1!A7,gab_soils_dev2!$R$2:$R$237,Sheet1!B7)</f>
         <v>6.4525499000000002</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>0.01</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <f t="shared" si="0"/>
         <v>6.4525499E-2</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="6">
         <f>SUM(E7:E10)/SUM($C$7:$C$10)</f>
         <v>3.7510834431987355E-2</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="1">
         <f t="shared" si="1"/>
         <v>6.4525499E-2</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="3">
         <f>SUM(G7:G10)/SUM(C7:C10)</f>
         <v>3.7510834431987355E-2</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="1">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="1">
         <f t="shared" si="3"/>
         <v>6.4525499000000002</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K7" s="3">
         <f>SUM(J7:J10)/SUM($C$7:$C$10)</f>
         <v>2.8343290628551983</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="1">
         <v>12.6</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M7" s="4">
         <f>L7*C7</f>
         <v>81.302128740000001</v>
       </c>
@@ -15277,151 +15479,151 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <f>SUMIFS(gab_soils_dev2!$S$2:$S$237,gab_soils_dev2!$N$2:$N$237,Sheet1!A8,gab_soils_dev2!$R$2:$R$237,Sheet1!B8)</f>
         <v>3.2108100000000001E-2</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="1">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="1">
         <f t="shared" si="3"/>
         <v>3.2108100000000001E-2</v>
       </c>
-      <c r="M8" s="2"/>
+      <c r="M8" s="4"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <f>SUMIFS(gab_soils_dev2!$S$2:$S$237,gab_soils_dev2!$N$2:$N$237,Sheet1!A9,gab_soils_dev2!$R$2:$R$237,Sheet1!B9)</f>
         <v>31.896553599999997</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>0.04</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <f t="shared" si="0"/>
         <v>1.275862144</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="1">
         <f t="shared" si="1"/>
         <v>1.275862144</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="1">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="1">
         <f t="shared" si="3"/>
         <v>95.689660799999984</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="1">
         <v>10.63</v>
       </c>
-      <c r="M9" s="2">
+      <c r="M9" s="4">
         <f>L9*C9</f>
         <v>339.060364768</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <f>SUMIFS(gab_soils_dev2!$S$2:$S$237,gab_soils_dev2!$N$2:$N$237,Sheet1!A10,gab_soils_dev2!$R$2:$R$237,Sheet1!B10)</f>
         <v>39.902380100000002</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>0.04</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <f t="shared" si="0"/>
         <v>1.596095204</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="1">
         <f t="shared" si="1"/>
         <v>1.596095204</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="1">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="1">
         <f t="shared" si="3"/>
         <v>119.70714030000001</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="1">
         <v>10.63</v>
       </c>
-      <c r="M10" s="2">
+      <c r="M10" s="4">
         <f>L10*C10</f>
         <v>424.16230046300007</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="M11" s="2"/>
+      <c r="M11" s="4"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <f>SUMIFS(gab_soils_dev2!$S$2:$S$237,gab_soils_dev2!$N$2:$N$237,Sheet1!A12,gab_soils_dev2!$R$2:$R$237,Sheet1!B12)</f>
         <v>5.4180948999999998</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>0.01</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="1">
         <f t="shared" si="0"/>
         <v>5.4180948999999999E-2</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="6">
         <f>SUM(E12:E16)/SUM($C$12:$C$16)</f>
         <v>2.8939130636948369E-2</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="1">
         <f t="shared" si="1"/>
         <v>5.4180948999999999E-2</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="3">
         <f>SUM(G12:G16)/SUM(C12:C16)</f>
         <v>2.8939130636948369E-2</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="1">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="1">
         <f t="shared" si="3"/>
         <v>5.4180948999999998</v>
       </c>
-      <c r="K12" s="1">
+      <c r="K12" s="3">
         <f>SUM(J12:J16)/SUM($C$12:$C$16)</f>
         <v>2.2494466825182342</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="1">
         <v>12.6</v>
       </c>
-      <c r="M12" s="2">
+      <c r="M12" s="4">
         <f>L12*C12</f>
         <v>68.267995739999989</v>
       </c>
@@ -15431,181 +15633,181 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <f>SUMIFS(gab_soils_dev2!$S$2:$S$237,gab_soils_dev2!$N$2:$N$237,Sheet1!A13,gab_soils_dev2!$R$2:$R$237,Sheet1!B13)</f>
         <v>7.8713898999999996</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <v>0.01</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="1">
         <f t="shared" si="0"/>
         <v>7.8713899000000004E-2</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="1">
         <f t="shared" si="1"/>
         <v>7.8713899000000004E-2</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="1">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="1">
         <f t="shared" si="3"/>
         <v>7.8713898999999996</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="1">
         <v>12.6</v>
       </c>
-      <c r="M13" s="2">
+      <c r="M13" s="4">
         <f>L13*C13</f>
         <v>99.179512739999993</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <f>SUMIFS(gab_soils_dev2!$S$2:$S$237,gab_soils_dev2!$N$2:$N$237,Sheet1!A14,gab_soils_dev2!$R$2:$R$237,Sheet1!B14)</f>
         <v>1.6603504000000002</v>
       </c>
-      <c r="M14" s="2"/>
+      <c r="M14" s="4"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <f>SUMIFS(gab_soils_dev2!$S$2:$S$237,gab_soils_dev2!$N$2:$N$237,Sheet1!A15,gab_soils_dev2!$R$2:$R$237,Sheet1!B15)</f>
         <v>6.0003853999999999</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="1">
         <v>0.04</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="1">
         <f t="shared" si="0"/>
         <v>0.24001541600000001</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="1">
         <f t="shared" si="1"/>
         <v>0.24001541600000001</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="1">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="1">
         <f t="shared" si="3"/>
         <v>18.0011562</v>
       </c>
-      <c r="L15">
+      <c r="L15" s="1">
         <v>10.63</v>
       </c>
-      <c r="M15" s="2">
+      <c r="M15" s="4">
         <f>L15*C15</f>
         <v>63.784096802000001</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
         <f>SUMIFS(gab_soils_dev2!$S$2:$S$237,gab_soils_dev2!$N$2:$N$237,Sheet1!A16,gab_soils_dev2!$R$2:$R$237,Sheet1!B16)</f>
         <v>21.098785199999998</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="1">
         <v>0.04</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="1">
         <f t="shared" si="0"/>
         <v>0.8439514079999999</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="1">
         <f t="shared" si="1"/>
         <v>0.8439514079999999</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="1">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="1">
         <f t="shared" si="3"/>
         <v>63.296355599999998</v>
       </c>
-      <c r="L16">
+      <c r="L16" s="1">
         <v>10.63</v>
       </c>
-      <c r="M16" s="2">
+      <c r="M16" s="4">
         <f>L16*C16</f>
         <v>224.280086676</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="M17" s="2"/>
+      <c r="M17" s="4"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="1">
         <f>SUMIFS(gab_soils_dev2!$S$2:$S$237,gab_soils_dev2!$N$2:$N$237,Sheet1!A18,gab_soils_dev2!$R$2:$R$237,Sheet1!B18)</f>
         <v>3.9844502999999998</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="1">
         <v>4.74</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="1">
         <f t="shared" si="0"/>
         <v>18.886294421999999</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="2">
         <f>SUM(E18:E27)/SUM($C$18:$C$27)</f>
         <v>0.31769948217616567</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="1">
         <f t="shared" si="1"/>
         <v>18.886294421999999</v>
       </c>
-      <c r="H18" s="1">
+      <c r="H18" s="3">
         <f>SUM(G18:G27)/SUM(C18:C27)</f>
         <v>0.31769948217616567</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="1">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="1">
         <f t="shared" si="3"/>
         <v>19.922251499999998</v>
       </c>
-      <c r="K18" s="1">
+      <c r="K18" s="3">
         <f>SUM(J18:J27)/SUM($C$18:$C$27)</f>
         <v>1.8496386012042261</v>
       </c>
-      <c r="L18">
+      <c r="L18" s="1">
         <v>1.93</v>
       </c>
-      <c r="M18" s="2">
+      <c r="M18" s="4">
         <f t="shared" ref="M18:M23" si="4">L18*C18</f>
         <v>7.6899890789999992</v>
       </c>
@@ -15615,371 +15817,371 @@
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="1">
         <f>SUMIFS(gab_soils_dev2!$S$2:$S$237,gab_soils_dev2!$N$2:$N$237,Sheet1!A19,gab_soils_dev2!$R$2:$R$237,Sheet1!B19)</f>
         <v>12.766520700000001</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="1">
         <v>0.04</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="1">
         <f t="shared" si="0"/>
         <v>0.51066082800000001</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="1">
         <f t="shared" si="1"/>
         <v>0.51066082800000001</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="1">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="J19">
+      <c r="J19" s="1">
         <f t="shared" si="3"/>
         <v>38.299562100000003</v>
       </c>
-      <c r="L19">
+      <c r="L19" s="1">
         <v>10.63</v>
       </c>
-      <c r="M19" s="2">
+      <c r="M19" s="4">
         <f t="shared" si="4"/>
         <v>135.70811504100001</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="1">
         <f>SUMIFS(gab_soils_dev2!$S$2:$S$237,gab_soils_dev2!$N$2:$N$237,Sheet1!A20,gab_soils_dev2!$R$2:$R$237,Sheet1!B20)</f>
         <v>0.52649130000000011</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="1">
         <v>0.04</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="1">
         <f t="shared" si="0"/>
         <v>2.1059652000000005E-2</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="1">
         <f t="shared" si="1"/>
         <v>2.1059652000000005E-2</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="1">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="J20">
+      <c r="J20" s="1">
         <f t="shared" si="3"/>
         <v>1.5794739000000004</v>
       </c>
-      <c r="L20">
+      <c r="L20" s="1">
         <v>10.63</v>
       </c>
-      <c r="M20" s="2">
+      <c r="M20" s="4">
         <f t="shared" si="4"/>
         <v>5.5966025190000019</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="1">
         <f>SUMIFS(gab_soils_dev2!$S$2:$S$237,gab_soils_dev2!$N$2:$N$237,Sheet1!A21,gab_soils_dev2!$R$2:$R$237,Sheet1!B21)</f>
         <v>0.38403999999999999</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="1">
         <v>0.04</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="1">
         <f t="shared" si="0"/>
         <v>1.53616E-2</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="1">
         <f t="shared" si="1"/>
         <v>1.53616E-2</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="1">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="J21">
+      <c r="J21" s="1">
         <f t="shared" si="3"/>
         <v>1.15212</v>
       </c>
-      <c r="L21">
+      <c r="L21" s="1">
         <v>10.63</v>
       </c>
-      <c r="M21" s="2">
+      <c r="M21" s="4">
         <f t="shared" si="4"/>
         <v>4.0823451999999998</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="1">
         <f>SUMIFS(gab_soils_dev2!$S$2:$S$237,gab_soils_dev2!$N$2:$N$237,Sheet1!A22,gab_soils_dev2!$R$2:$R$237,Sheet1!B22)</f>
         <v>0.85415600000000003</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="1">
         <v>0.01</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="1">
         <f t="shared" si="0"/>
         <v>8.5415600000000001E-3</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="1">
         <f t="shared" si="1"/>
         <v>8.5415600000000001E-3</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="1">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="J22">
+      <c r="J22" s="1">
         <f t="shared" si="3"/>
         <v>0.85415600000000003</v>
       </c>
-      <c r="L22">
+      <c r="L22" s="1">
         <v>12.6</v>
       </c>
-      <c r="M22" s="2">
+      <c r="M22" s="4">
         <f t="shared" si="4"/>
         <v>10.762365600000001</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="1">
         <f>SUMIFS(gab_soils_dev2!$S$2:$S$237,gab_soils_dev2!$N$2:$N$237,Sheet1!A23,gab_soils_dev2!$R$2:$R$237,Sheet1!B23)</f>
         <v>39.019436499999998</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="1">
         <v>0.01</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="1">
         <f t="shared" si="0"/>
         <v>0.39019436499999999</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="1">
         <f t="shared" si="1"/>
         <v>0.39019436499999999</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="1">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="J23">
+      <c r="J23" s="1">
         <f t="shared" si="3"/>
         <v>39.019436499999998</v>
       </c>
-      <c r="L23">
+      <c r="L23" s="1">
         <v>12.6</v>
       </c>
-      <c r="M23" s="2">
+      <c r="M23" s="4">
         <f t="shared" si="4"/>
         <v>491.64489989999998</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="1">
         <f>SUMIFS(gab_soils_dev2!$S$2:$S$237,gab_soils_dev2!$N$2:$N$237,Sheet1!A24,gab_soils_dev2!$R$2:$R$237,Sheet1!B24)</f>
         <v>0.26601599999999997</v>
       </c>
-      <c r="M24" s="2"/>
+      <c r="M24" s="4"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="1">
         <f>SUMIFS(gab_soils_dev2!$S$2:$S$237,gab_soils_dev2!$N$2:$N$237,Sheet1!A25,gab_soils_dev2!$R$2:$R$237,Sheet1!B25)</f>
         <v>5.1600298999999996</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="1">
         <v>0.04</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="1">
         <f t="shared" si="0"/>
         <v>0.20640119599999998</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="1">
         <f t="shared" si="1"/>
         <v>0.20640119599999998</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="1">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="J25">
+      <c r="J25" s="1">
         <f t="shared" si="3"/>
         <v>15.480089699999999</v>
       </c>
-      <c r="L25">
+      <c r="L25" s="1">
         <v>10.63</v>
       </c>
-      <c r="M25" s="2">
+      <c r="M25" s="4">
         <f>L25*C25</f>
         <v>54.851117836999997</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="1">
         <f>SUMIFS(gab_soils_dev2!$S$2:$S$237,gab_soils_dev2!$N$2:$N$237,Sheet1!A26,gab_soils_dev2!$R$2:$R$237,Sheet1!B26)</f>
         <v>3.6584100000000001E-2</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="1">
         <v>0.04</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="1">
         <f t="shared" si="0"/>
         <v>1.463364E-3</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="1">
         <f t="shared" si="1"/>
         <v>1.463364E-3</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="1">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="J26">
+      <c r="J26" s="1">
         <f t="shared" si="3"/>
         <v>0.1097523</v>
       </c>
-      <c r="L26">
+      <c r="L26" s="1">
         <v>10.63</v>
       </c>
-      <c r="M26" s="2">
+      <c r="M26" s="4">
         <f>L26*C26</f>
         <v>0.38888898300000002</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="1">
         <f>SUMIFS(gab_soils_dev2!$S$2:$S$237,gab_soils_dev2!$N$2:$N$237,Sheet1!A27,gab_soils_dev2!$R$2:$R$237,Sheet1!B27)</f>
         <v>9.2302800000000004E-2</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="1">
         <v>0.04</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="1">
         <f t="shared" si="0"/>
         <v>3.6921120000000004E-3</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="1">
         <f t="shared" si="1"/>
         <v>3.6921120000000004E-3</v>
       </c>
-      <c r="I27">
+      <c r="I27" s="1">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="J27">
+      <c r="J27" s="1">
         <f t="shared" si="3"/>
         <v>0.2769084</v>
       </c>
-      <c r="L27">
+      <c r="L27" s="1">
         <v>10.63</v>
       </c>
-      <c r="M27" s="2">
+      <c r="M27" s="4">
         <f>L27*C27</f>
         <v>0.98117876400000015</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="M28" s="2"/>
+      <c r="M28" s="4"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="1">
         <f>SUMIFS(gab_soils_dev2!$S$2:$S$237,gab_soils_dev2!$N$2:$N$237,Sheet1!A29,gab_soils_dev2!$R$2:$R$237,Sheet1!B29)</f>
         <v>14.829930099999999</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="1">
         <v>0.04</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="1">
         <f t="shared" si="0"/>
         <v>0.59319720399999998</v>
       </c>
-      <c r="F29" s="3">
+      <c r="F29" s="6">
         <f>SUM(E29:E34)/SUM($C$29:$C$34)</f>
         <v>3.9994557303115033E-2</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="1">
         <f t="shared" si="1"/>
         <v>0.59319720399999998</v>
       </c>
-      <c r="H29" s="1">
+      <c r="H29" s="3">
         <f>SUM(G29:G34)/SUM(C29:C34)</f>
         <v>3.9994557303115033E-2</v>
       </c>
-      <c r="I29">
+      <c r="I29" s="1">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="J29">
+      <c r="J29" s="1">
         <f t="shared" si="3"/>
         <v>44.489790299999996</v>
       </c>
-      <c r="K29" s="1">
+      <c r="K29" s="3">
         <f>SUM(J29:J34)/SUM($C$29:$C$34)</f>
         <v>2.9996371535410016</v>
       </c>
-      <c r="L29">
+      <c r="L29" s="1">
         <v>10.63</v>
       </c>
-      <c r="M29" s="2">
+      <c r="M29" s="4">
         <f t="shared" ref="M29:M34" si="5">L29*C29</f>
         <v>157.64215696299999</v>
       </c>
@@ -15989,244 +16191,244 @@
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="1">
         <f>SUMIFS(gab_soils_dev2!$S$2:$S$237,gab_soils_dev2!$N$2:$N$237,Sheet1!A30,gab_soils_dev2!$R$2:$R$237,Sheet1!B30)</f>
         <v>0.90576279999999998</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="1">
         <v>0.04</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="1">
         <f t="shared" si="0"/>
         <v>3.6230511999999999E-2</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="1">
         <f t="shared" si="1"/>
         <v>3.6230511999999999E-2</v>
       </c>
-      <c r="I30">
+      <c r="I30" s="1">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="J30">
+      <c r="J30" s="1">
         <f t="shared" si="3"/>
         <v>2.7172884000000002</v>
       </c>
-      <c r="L30">
+      <c r="L30" s="1">
         <v>10.63</v>
       </c>
-      <c r="M30" s="2">
+      <c r="M30" s="4">
         <f t="shared" si="5"/>
         <v>9.6282585640000011</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="1">
         <f>SUMIFS(gab_soils_dev2!$S$2:$S$237,gab_soils_dev2!$N$2:$N$237,Sheet1!A31,gab_soils_dev2!$R$2:$R$237,Sheet1!B31)</f>
         <v>0.31746519999999995</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="1">
         <v>0.04</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="1">
         <f t="shared" si="0"/>
         <v>1.2698607999999998E-2</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="1">
         <f t="shared" si="1"/>
         <v>1.2698607999999998E-2</v>
       </c>
-      <c r="I31">
+      <c r="I31" s="1">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="J31">
+      <c r="J31" s="1">
         <f t="shared" si="3"/>
         <v>0.95239559999999979</v>
       </c>
-      <c r="L31">
+      <c r="L31" s="1">
         <v>10.63</v>
       </c>
-      <c r="M31" s="2">
+      <c r="M31" s="4">
         <f t="shared" si="5"/>
         <v>3.3746550759999998</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="1">
         <f>SUMIFS(gab_soils_dev2!$S$2:$S$237,gab_soils_dev2!$N$2:$N$237,Sheet1!A32,gab_soils_dev2!$R$2:$R$237,Sheet1!B32)</f>
         <v>9.3691E-3</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="1">
         <v>0.01</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="1">
         <f t="shared" si="0"/>
         <v>9.3691000000000008E-5</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="1">
         <f t="shared" si="1"/>
         <v>9.3691000000000008E-5</v>
       </c>
-      <c r="I32">
+      <c r="I32" s="1">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="J32">
+      <c r="J32" s="1">
         <f t="shared" si="3"/>
         <v>9.3691E-3</v>
       </c>
-      <c r="L32">
+      <c r="L32" s="1">
         <v>12.6</v>
       </c>
-      <c r="M32" s="2">
+      <c r="M32" s="4">
         <f t="shared" si="5"/>
         <v>0.11805066</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="A33" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="1">
         <f>SUMIFS(gab_soils_dev2!$S$2:$S$237,gab_soils_dev2!$N$2:$N$237,Sheet1!A33,gab_soils_dev2!$R$2:$R$237,Sheet1!B33)</f>
         <v>20.548353800000001</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="1">
         <v>0.04</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="1">
         <f t="shared" si="0"/>
         <v>0.82193415200000008</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="1">
         <f t="shared" si="1"/>
         <v>0.82193415200000008</v>
       </c>
-      <c r="I33">
+      <c r="I33" s="1">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="J33">
+      <c r="J33" s="1">
         <f t="shared" si="3"/>
         <v>61.645061400000003</v>
       </c>
-      <c r="L33">
+      <c r="L33" s="1">
         <v>10.63</v>
       </c>
-      <c r="M33" s="2">
+      <c r="M33" s="4">
         <f t="shared" si="5"/>
         <v>218.42900089400004</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="A34" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="1">
         <f>SUMIFS(gab_soils_dev2!$S$2:$S$237,gab_soils_dev2!$N$2:$N$237,Sheet1!A34,gab_soils_dev2!$R$2:$R$237,Sheet1!B34)</f>
         <v>15.0313482</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="1">
         <v>0.04</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="1">
         <f t="shared" si="0"/>
         <v>0.60125392799999999</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="1">
         <f t="shared" si="1"/>
         <v>0.60125392799999999</v>
       </c>
-      <c r="I34">
+      <c r="I34" s="1">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="J34">
+      <c r="J34" s="1">
         <f t="shared" si="3"/>
         <v>45.094044600000004</v>
       </c>
-      <c r="L34">
+      <c r="L34" s="1">
         <v>10.63</v>
       </c>
-      <c r="M34" s="2">
+      <c r="M34" s="4">
         <f t="shared" si="5"/>
         <v>159.78323136600002</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="M35" s="2"/>
+      <c r="M35" s="4"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="A36" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="1">
         <f>SUMIFS(gab_soils_dev2!$S$2:$S$237,gab_soils_dev2!$N$2:$N$237,Sheet1!A36,gab_soils_dev2!$R$2:$R$237,Sheet1!B36)</f>
         <v>7.0418455999999994</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="1">
         <v>0.04</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="1">
         <f t="shared" si="0"/>
         <v>0.28167382399999996</v>
       </c>
-      <c r="F36" s="3">
+      <c r="F36" s="6">
         <f>SUM(E36:E44)/SUM($C$36:$C$44)</f>
         <v>3.3087604272505587E-2</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="1">
         <f t="shared" si="1"/>
         <v>0.28167382399999996</v>
       </c>
-      <c r="H36" s="1">
+      <c r="H36" s="3">
         <f>SUM(G36:G44)/SUM(C36:C44)</f>
         <v>3.3087604272505587E-2</v>
       </c>
-      <c r="I36">
+      <c r="I36" s="1">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="J36">
+      <c r="J36" s="1">
         <f t="shared" si="3"/>
         <v>21.125536799999999</v>
       </c>
-      <c r="K36" s="1">
+      <c r="K36" s="3">
         <f>SUM(J36:J44)/SUM($C$36:$C$44)</f>
         <v>2.5377652593530771</v>
       </c>
-      <c r="L36">
+      <c r="L36" s="1">
         <v>10.63</v>
       </c>
-      <c r="M36" s="2">
+      <c r="M36" s="4">
         <f>L36*C36</f>
         <v>74.854818727999998</v>
       </c>
@@ -16236,286 +16438,2235 @@
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="A37" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="1">
         <f>SUMIFS(gab_soils_dev2!$S$2:$S$237,gab_soils_dev2!$N$2:$N$237,Sheet1!A37,gab_soils_dev2!$R$2:$R$237,Sheet1!B37)</f>
         <v>0.64609630000000007</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="1">
         <v>0.04</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="1">
         <f t="shared" si="0"/>
         <v>2.5843852000000004E-2</v>
       </c>
-      <c r="G37">
+      <c r="G37" s="1">
         <f t="shared" si="1"/>
         <v>2.5843852000000004E-2</v>
       </c>
-      <c r="I37">
+      <c r="I37" s="1">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="J37">
+      <c r="J37" s="1">
         <f t="shared" si="3"/>
         <v>1.9382889000000003</v>
       </c>
-      <c r="L37">
+      <c r="L37" s="1">
         <v>10.63</v>
       </c>
-      <c r="M37" s="2">
+      <c r="M37" s="4">
         <f>L37*C37</f>
         <v>6.868003669000001</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="A38" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="1">
         <f>SUMIFS(gab_soils_dev2!$S$2:$S$237,gab_soils_dev2!$N$2:$N$237,Sheet1!A38,gab_soils_dev2!$R$2:$R$237,Sheet1!B38)</f>
         <v>3.2390000000000001E-4</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="1">
         <v>0.04</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="1">
         <f t="shared" si="0"/>
         <v>1.2956000000000001E-5</v>
       </c>
-      <c r="G38">
+      <c r="G38" s="1">
         <f t="shared" si="1"/>
         <v>1.2956000000000001E-5</v>
       </c>
-      <c r="I38">
+      <c r="I38" s="1">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="J38">
+      <c r="J38" s="1">
         <f t="shared" si="3"/>
         <v>9.7170000000000004E-4</v>
       </c>
-      <c r="L38">
+      <c r="L38" s="1">
         <v>10.63</v>
       </c>
-      <c r="M38" s="2">
+      <c r="M38" s="4">
         <f>L38*C38</f>
         <v>3.4430570000000002E-3</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="A39" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="1">
         <f>SUMIFS(gab_soils_dev2!$S$2:$S$237,gab_soils_dev2!$N$2:$N$237,Sheet1!A39,gab_soils_dev2!$R$2:$R$237,Sheet1!B39)</f>
         <v>29.750965900000001</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="1">
         <v>0.01</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="1">
         <f t="shared" si="0"/>
         <v>0.29750965900000004</v>
       </c>
-      <c r="G39">
+      <c r="G39" s="1">
         <f t="shared" si="1"/>
         <v>0.29750965900000004</v>
       </c>
-      <c r="I39">
+      <c r="I39" s="1">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="J39">
+      <c r="J39" s="1">
         <f t="shared" si="3"/>
         <v>29.750965900000001</v>
       </c>
-      <c r="L39">
+      <c r="L39" s="1">
         <v>12.6</v>
       </c>
-      <c r="M39" s="2">
+      <c r="M39" s="4">
         <f>L39*C39</f>
         <v>374.86217033999998</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="A40" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="1">
         <f>SUMIFS(gab_soils_dev2!$S$2:$S$237,gab_soils_dev2!$N$2:$N$237,Sheet1!A40,gab_soils_dev2!$R$2:$R$237,Sheet1!B40)</f>
         <v>2.8935398999999999</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="1">
         <v>0.01</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="1">
         <f t="shared" si="0"/>
         <v>2.8935399000000001E-2</v>
       </c>
-      <c r="G40">
+      <c r="G40" s="1">
         <f t="shared" si="1"/>
         <v>2.8935399000000001E-2</v>
       </c>
-      <c r="I40">
+      <c r="I40" s="1">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="J40">
+      <c r="J40" s="1">
         <f t="shared" si="3"/>
         <v>2.8935398999999999</v>
       </c>
-      <c r="L40">
+      <c r="L40" s="1">
         <v>12.6</v>
       </c>
-      <c r="M40" s="2">
+      <c r="M40" s="4">
         <f>L40*C40</f>
         <v>36.458602739999996</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="A41" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="1">
         <f>SUMIFS(gab_soils_dev2!$S$2:$S$237,gab_soils_dev2!$N$2:$N$237,Sheet1!A41,gab_soils_dev2!$R$2:$R$237,Sheet1!B41)</f>
         <v>0.6136029999999999</v>
       </c>
-      <c r="M41" s="2"/>
+      <c r="M41" s="4"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="A42" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="1">
         <f>SUMIFS(gab_soils_dev2!$S$2:$S$237,gab_soils_dev2!$N$2:$N$237,Sheet1!A42,gab_soils_dev2!$R$2:$R$237,Sheet1!B42)</f>
         <v>1.4298199</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="1">
         <v>0.04</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="1">
         <f t="shared" si="0"/>
         <v>5.7192796000000004E-2</v>
       </c>
-      <c r="G42">
+      <c r="G42" s="1">
         <f t="shared" si="1"/>
         <v>5.7192796000000004E-2</v>
       </c>
-      <c r="I42">
+      <c r="I42" s="1">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="J42">
+      <c r="J42" s="1">
         <f t="shared" si="3"/>
         <v>4.2894597000000001</v>
       </c>
-      <c r="L42">
+      <c r="L42" s="1">
         <v>10.63</v>
       </c>
-      <c r="M42" s="2">
+      <c r="M42" s="4">
         <f>L42*C42</f>
         <v>15.198985537000002</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="A43" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="1">
         <f>SUMIFS(gab_soils_dev2!$S$2:$S$237,gab_soils_dev2!$N$2:$N$237,Sheet1!A43,gab_soils_dev2!$R$2:$R$237,Sheet1!B43)</f>
         <v>50.643296200000009</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="1">
         <v>0.04</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="1">
         <f t="shared" si="0"/>
         <v>2.0257318480000004</v>
       </c>
-      <c r="G43">
+      <c r="G43" s="1">
         <f t="shared" si="1"/>
         <v>2.0257318480000004</v>
       </c>
-      <c r="I43">
+      <c r="I43" s="1">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="J43">
+      <c r="J43" s="1">
         <f t="shared" si="3"/>
         <v>151.92988860000003</v>
       </c>
-      <c r="L43">
+      <c r="L43" s="1">
         <v>10.63</v>
       </c>
-      <c r="M43" s="2">
+      <c r="M43" s="4">
         <f>L43*C43</f>
         <v>538.33823860600012</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="A44" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="1">
         <f>SUMIFS(gab_soils_dev2!$S$2:$S$237,gab_soils_dev2!$N$2:$N$237,Sheet1!A44,gab_soils_dev2!$R$2:$R$237,Sheet1!B44)</f>
         <v>52.209361000000001</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="1">
         <v>0.04</v>
       </c>
-      <c r="E44">
+      <c r="E44" s="1">
         <f t="shared" si="0"/>
         <v>2.0883744399999999</v>
       </c>
-      <c r="G44">
+      <c r="G44" s="1">
         <f t="shared" si="1"/>
         <v>2.0883744399999999</v>
       </c>
-      <c r="I44">
+      <c r="I44" s="1">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="J44">
+      <c r="J44" s="1">
         <f t="shared" si="3"/>
         <v>156.628083</v>
       </c>
-      <c r="L44">
+      <c r="L44" s="1">
         <v>10.63</v>
       </c>
-      <c r="M44" s="2">
+      <c r="M44" s="4">
         <f>L44*C44</f>
         <v>554.9855074300001</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="M45" s="2"/>
+      <c r="M45" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q11"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="41.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2">
+        <f>SUMIF(Sheet1!$B$2:$B$44,Sheet2!A2,Sheet1!$C$2:$C$44)</f>
+        <v>6.7644836999999995</v>
+      </c>
+      <c r="C2">
+        <v>4.74</v>
+      </c>
+      <c r="D2">
+        <v>1.93</v>
+      </c>
+      <c r="E2">
+        <v>0.437</v>
+      </c>
+      <c r="F2">
+        <v>6.2E-2</v>
+      </c>
+      <c r="G2">
+        <v>2.4E-2</v>
+      </c>
+      <c r="H2">
+        <f>$B$2*C2</f>
+        <v>32.063652738000002</v>
+      </c>
+      <c r="I2">
+        <f t="shared" ref="I2:L2" si="0">$B$2*D2</f>
+        <v>13.055453540999999</v>
+      </c>
+      <c r="J2">
+        <f t="shared" si="0"/>
+        <v>2.9560793769</v>
+      </c>
+      <c r="K2">
+        <f t="shared" si="0"/>
+        <v>0.41939798939999995</v>
+      </c>
+      <c r="L2">
+        <f t="shared" si="0"/>
+        <v>0.16234760879999999</v>
+      </c>
+      <c r="M2" s="7">
+        <f>SUM(H2:H11)/SUM($B$2:$B$11)</f>
+        <v>0.10085043132569926</v>
+      </c>
+      <c r="N2" s="8">
+        <f t="shared" ref="N2:Q2" si="1">SUM(I2:I11)/SUM($B$2:$B$11)</f>
+        <v>9.6238356870185626</v>
+      </c>
+      <c r="O2" s="7">
+        <f t="shared" si="1"/>
+        <v>0.46471264829509912</v>
+      </c>
+      <c r="P2" s="7">
+        <f t="shared" si="1"/>
+        <v>0.3279629675191314</v>
+      </c>
+      <c r="Q2" s="7">
+        <f t="shared" si="1"/>
+        <v>0.21042611345320822</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3">
+        <f>SUMIF(Sheet1!$B$2:$B$44,Sheet2!A3,Sheet1!$C$2:$C$44)</f>
+        <v>117.89898379999998</v>
+      </c>
+      <c r="C3">
+        <v>0.01</v>
+      </c>
+      <c r="D3">
+        <v>12.6</v>
+      </c>
+      <c r="E3">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="F3">
+        <v>0.378</v>
+      </c>
+      <c r="G3">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="H3">
+        <f>$B$3*C3</f>
+        <v>1.1789898379999999</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:L3" si="2">$B$3*D3</f>
+        <v>1485.5271958799997</v>
+      </c>
+      <c r="J3">
+        <f t="shared" si="2"/>
+        <v>56.002017304999988</v>
+      </c>
+      <c r="K3">
+        <f t="shared" si="2"/>
+        <v>44.565815876399995</v>
+      </c>
+      <c r="L3">
+        <f t="shared" si="2"/>
+        <v>31.243230706999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <f>SUMIF(Sheet1!$B$2:$B$44,Sheet2!A4,Sheet1!$C$2:$C$44)</f>
+        <v>109.27343060000001</v>
+      </c>
+      <c r="C4">
+        <v>0.04</v>
+      </c>
+      <c r="D4">
+        <v>8.27</v>
+      </c>
+      <c r="E4">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="F4">
+        <v>0.31</v>
+      </c>
+      <c r="G4">
+        <v>0.187</v>
+      </c>
+      <c r="H4">
+        <f>$B$4*C4</f>
+        <v>4.3709372240000004</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ref="I4:L4" si="3">$B$4*D4</f>
+        <v>903.69127106200006</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="3"/>
+        <v>50.702871798400011</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="3"/>
+        <v>33.874763486000006</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="3"/>
+        <v>20.434131522200001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5">
+        <f>SUMIF(Sheet1!$B$2:$B$44,Sheet2!A5,Sheet1!$C$2:$C$44)</f>
+        <v>128.3622325</v>
+      </c>
+      <c r="C5">
+        <v>0.04</v>
+      </c>
+      <c r="D5">
+        <v>8.27</v>
+      </c>
+      <c r="E5">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="F5">
+        <v>0.31</v>
+      </c>
+      <c r="G5">
+        <v>0.187</v>
+      </c>
+      <c r="H5">
+        <f>$B$5*C5</f>
+        <v>5.1344893000000003</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ref="I5:L5" si="4">$B$5*D5</f>
+        <v>1061.555662775</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="4"/>
+        <v>59.560075880000007</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="4"/>
+        <v>39.792292074999999</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="4"/>
+        <v>24.0037374775</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6">
+        <f>SUMIF(Sheet1!$B$2:$B$44,Sheet2!A6,Sheet1!$C$2:$C$44)</f>
+        <v>2.5720775000000002</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <f>$B$6*C6</f>
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <f t="shared" ref="I6:L6" si="5">$B$6*D6</f>
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7">
+        <f>SUMIF(Sheet1!$B$2:$B$44,Sheet2!A7,Sheet1!$C$2:$C$44)</f>
+        <v>36.0232168</v>
+      </c>
+      <c r="C7">
+        <v>0.01</v>
+      </c>
+      <c r="D7">
+        <v>12.6</v>
+      </c>
+      <c r="E7">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="F7">
+        <v>0.378</v>
+      </c>
+      <c r="G7">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="H7">
+        <f>$B$7*C7</f>
+        <v>0.36023216800000002</v>
+      </c>
+      <c r="I7">
+        <f t="shared" ref="I7:L7" si="6">$B$7*D7</f>
+        <v>453.89253167999999</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="6"/>
+        <v>17.111027979999999</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="6"/>
+        <v>13.616775950400001</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="6"/>
+        <v>9.5461524520000012</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8">
+        <f>SUMIF(Sheet1!$B$2:$B$44,Sheet2!A8,Sheet1!$C$2:$C$44)</f>
+        <v>34.638296400000002</v>
+      </c>
+      <c r="C8">
+        <v>0.04</v>
+      </c>
+      <c r="D8">
+        <v>8.27</v>
+      </c>
+      <c r="E8">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="F8">
+        <v>0.31</v>
+      </c>
+      <c r="G8">
+        <v>0.187</v>
+      </c>
+      <c r="H8">
+        <f>$B$8*C8</f>
+        <v>1.3855318560000001</v>
+      </c>
+      <c r="I8">
+        <f t="shared" ref="I8:L8" si="7">$B$8*D8</f>
+        <v>286.45871122799997</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="7"/>
+        <v>16.0721695296</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="7"/>
+        <v>10.737871884</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="7"/>
+        <v>6.4773614267999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9">
+        <f>SUMIF(Sheet1!$B$2:$B$44,Sheet2!A9,Sheet1!$C$2:$C$44)</f>
+        <v>2.0783504000000002</v>
+      </c>
+      <c r="C9">
+        <v>0.04</v>
+      </c>
+      <c r="D9">
+        <v>8.27</v>
+      </c>
+      <c r="E9">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="F9">
+        <v>0.31</v>
+      </c>
+      <c r="G9">
+        <v>0.187</v>
+      </c>
+      <c r="H9">
+        <f>$B$9*C9</f>
+        <v>8.3134016000000005E-2</v>
+      </c>
+      <c r="I9">
+        <f t="shared" ref="I9:L9" si="8">$B$9*D9</f>
+        <v>17.187957808</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="8"/>
+        <v>0.96435458560000009</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="8"/>
+        <v>0.64428862400000009</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="8"/>
+        <v>0.38865152480000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10">
+        <f>SUMIF(Sheet1!$B$2:$B$44,Sheet2!A10,Sheet1!$C$2:$C$44)</f>
+        <v>0.70182909999999998</v>
+      </c>
+      <c r="C10">
+        <v>0.04</v>
+      </c>
+      <c r="D10">
+        <v>8.27</v>
+      </c>
+      <c r="E10">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="F10">
+        <v>0.31</v>
+      </c>
+      <c r="G10">
+        <v>0.187</v>
+      </c>
+      <c r="H10">
+        <f>$B$10*C10</f>
+        <v>2.8073164000000001E-2</v>
+      </c>
+      <c r="I10">
+        <f t="shared" ref="I10:L10" si="9">$B$10*D10</f>
+        <v>5.8041266569999994</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="9"/>
+        <v>0.32564870239999999</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="9"/>
+        <v>0.217567021</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="9"/>
+        <v>0.13124204170000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11">
+        <f>SUMIF(Sheet1!$B$2:$B$44,Sheet2!A11,Sheet1!$C$2:$C$44)</f>
+        <v>6.5898497999999996</v>
+      </c>
+      <c r="C11">
+        <v>0.04</v>
+      </c>
+      <c r="D11">
+        <v>8.27</v>
+      </c>
+      <c r="E11">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="F11">
+        <v>0.31</v>
+      </c>
+      <c r="G11">
+        <v>0.187</v>
+      </c>
+      <c r="H11">
+        <f>$B$11*C11</f>
+        <v>0.263593992</v>
+      </c>
+      <c r="I11">
+        <f t="shared" ref="I11:L11" si="10">$B$11*D11</f>
+        <v>54.498057845999995</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="10"/>
+        <v>3.0576903072000001</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="10"/>
+        <v>2.0428534379999999</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="10"/>
+        <v>1.2323019125999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H31"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.28515625" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4">
+        <v>72</v>
+      </c>
+      <c r="C4" s="9">
+        <f>5*3.281+B4</f>
+        <v>88.405000000000001</v>
+      </c>
+      <c r="D4" s="9">
+        <f>C4-5</f>
+        <v>83.405000000000001</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5" s="9">
+        <f t="shared" ref="C5:C31" si="0">5*3.281+B5</f>
+        <v>26.405000000000001</v>
+      </c>
+      <c r="D5" s="9">
+        <f t="shared" ref="D5:D31" si="1">C5-5</f>
+        <v>21.405000000000001</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6">
+        <v>13</v>
+      </c>
+      <c r="C6" s="9">
+        <f t="shared" si="0"/>
+        <v>29.405000000000001</v>
+      </c>
+      <c r="D6" s="9">
+        <f t="shared" si="1"/>
+        <v>24.405000000000001</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7">
+        <v>13</v>
+      </c>
+      <c r="C7" s="9">
+        <f t="shared" si="0"/>
+        <v>29.405000000000001</v>
+      </c>
+      <c r="D7" s="9">
+        <f t="shared" si="1"/>
+        <v>24.405000000000001</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8">
+        <v>16</v>
+      </c>
+      <c r="C8" s="9">
+        <f t="shared" si="0"/>
+        <v>32.405000000000001</v>
+      </c>
+      <c r="D8" s="9">
+        <f t="shared" si="1"/>
+        <v>27.405000000000001</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9">
+        <v>13</v>
+      </c>
+      <c r="C9" s="9">
+        <f t="shared" si="0"/>
+        <v>29.405000000000001</v>
+      </c>
+      <c r="D9" s="9">
+        <f t="shared" si="1"/>
+        <v>24.405000000000001</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10">
+        <v>13</v>
+      </c>
+      <c r="C10" s="9">
+        <f t="shared" si="0"/>
+        <v>29.405000000000001</v>
+      </c>
+      <c r="D10" s="9">
+        <f t="shared" si="1"/>
+        <v>24.405000000000001</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11">
+        <v>33</v>
+      </c>
+      <c r="C11" s="9">
+        <f t="shared" si="0"/>
+        <v>49.405000000000001</v>
+      </c>
+      <c r="D11" s="9">
+        <f t="shared" si="1"/>
+        <v>44.405000000000001</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12">
+        <v>52</v>
+      </c>
+      <c r="C12" s="9">
+        <f t="shared" si="0"/>
+        <v>68.405000000000001</v>
+      </c>
+      <c r="D12" s="9">
+        <f t="shared" si="1"/>
+        <v>63.405000000000001</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13">
+        <v>13</v>
+      </c>
+      <c r="C13" s="9">
+        <f t="shared" si="0"/>
+        <v>29.405000000000001</v>
+      </c>
+      <c r="D13" s="9">
+        <f t="shared" si="1"/>
+        <v>24.405000000000001</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14">
+        <v>115</v>
+      </c>
+      <c r="C14" s="9">
+        <f t="shared" si="0"/>
+        <v>131.405</v>
+      </c>
+      <c r="D14" s="9">
+        <f t="shared" si="1"/>
+        <v>126.405</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15">
+        <v>115</v>
+      </c>
+      <c r="C15" s="9">
+        <f t="shared" si="0"/>
+        <v>131.405</v>
+      </c>
+      <c r="D15" s="9">
+        <f t="shared" si="1"/>
+        <v>126.405</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16">
+        <v>33</v>
+      </c>
+      <c r="C16" s="9">
+        <f t="shared" si="0"/>
+        <v>49.405000000000001</v>
+      </c>
+      <c r="D16" s="9">
+        <f t="shared" si="1"/>
+        <v>44.405000000000001</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17">
+        <v>56</v>
+      </c>
+      <c r="C17" s="9">
+        <f t="shared" si="0"/>
+        <v>72.405000000000001</v>
+      </c>
+      <c r="D17" s="9">
+        <f t="shared" si="1"/>
+        <v>67.405000000000001</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18">
+        <v>148</v>
+      </c>
+      <c r="C18" s="9">
+        <f t="shared" si="0"/>
+        <v>164.405</v>
+      </c>
+      <c r="D18" s="9">
+        <f t="shared" si="1"/>
+        <v>159.405</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19">
+        <v>30</v>
+      </c>
+      <c r="C19" s="9">
+        <f t="shared" si="0"/>
+        <v>46.405000000000001</v>
+      </c>
+      <c r="D19" s="9">
+        <f t="shared" si="1"/>
+        <v>41.405000000000001</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20">
+        <v>10</v>
+      </c>
+      <c r="C20" s="9">
+        <f t="shared" si="0"/>
+        <v>26.405000000000001</v>
+      </c>
+      <c r="D20" s="9">
+        <f t="shared" si="1"/>
+        <v>21.405000000000001</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21">
+        <v>197</v>
+      </c>
+      <c r="C21" s="9">
+        <f t="shared" si="0"/>
+        <v>213.405</v>
+      </c>
+      <c r="D21" s="9">
+        <f t="shared" si="1"/>
+        <v>208.405</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22">
+        <v>180</v>
+      </c>
+      <c r="C22" s="9">
+        <f t="shared" si="0"/>
+        <v>196.405</v>
+      </c>
+      <c r="D22" s="9">
+        <f t="shared" si="1"/>
+        <v>191.405</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23">
+        <v>13</v>
+      </c>
+      <c r="C23" s="9">
+        <f t="shared" si="0"/>
+        <v>29.405000000000001</v>
+      </c>
+      <c r="D23" s="9">
+        <f t="shared" si="1"/>
+        <v>24.405000000000001</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24">
+        <v>13</v>
+      </c>
+      <c r="C24" s="9">
+        <f t="shared" si="0"/>
+        <v>29.405000000000001</v>
+      </c>
+      <c r="D24" s="9">
+        <f t="shared" si="1"/>
+        <v>24.405000000000001</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25">
+        <v>98</v>
+      </c>
+      <c r="C25" s="9">
+        <f t="shared" si="0"/>
+        <v>114.405</v>
+      </c>
+      <c r="D25" s="9">
+        <f t="shared" si="1"/>
+        <v>109.405</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26">
+        <v>36</v>
+      </c>
+      <c r="C26" s="9">
+        <f t="shared" si="0"/>
+        <v>52.405000000000001</v>
+      </c>
+      <c r="D26" s="9">
+        <f t="shared" si="1"/>
+        <v>47.405000000000001</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27">
+        <v>20</v>
+      </c>
+      <c r="C27" s="9">
+        <f t="shared" si="0"/>
+        <v>36.405000000000001</v>
+      </c>
+      <c r="D27" s="9">
+        <f t="shared" si="1"/>
+        <v>31.405000000000001</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>83</v>
+      </c>
+      <c r="B28">
+        <v>20</v>
+      </c>
+      <c r="C28" s="9">
+        <f t="shared" si="0"/>
+        <v>36.405000000000001</v>
+      </c>
+      <c r="D28" s="9">
+        <f t="shared" si="1"/>
+        <v>31.405000000000001</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29">
+        <v>20</v>
+      </c>
+      <c r="C29" s="9">
+        <f t="shared" si="0"/>
+        <v>36.405000000000001</v>
+      </c>
+      <c r="D29" s="9">
+        <f t="shared" si="1"/>
+        <v>31.405000000000001</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30">
+        <v>10</v>
+      </c>
+      <c r="C30" s="9">
+        <f t="shared" si="0"/>
+        <v>26.405000000000001</v>
+      </c>
+      <c r="D30" s="9">
+        <f t="shared" si="1"/>
+        <v>21.405000000000001</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31">
+        <v>180</v>
+      </c>
+      <c r="C31" s="9">
+        <f t="shared" si="0"/>
+        <v>196.405</v>
+      </c>
+      <c r="D31" s="9">
+        <f t="shared" si="1"/>
+        <v>191.405</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1">
+        <v>40</v>
+      </c>
+      <c r="C1" s="9">
+        <f>B1*3.28084</f>
+        <v>131.2336</v>
+      </c>
+      <c r="D1" s="9">
+        <f>C1-4</f>
+        <v>127.2336</v>
+      </c>
+      <c r="F1">
+        <v>7.2</v>
+      </c>
+      <c r="G1" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>40</v>
+      </c>
+      <c r="C2" s="9">
+        <f t="shared" ref="C2:C24" si="0">B2*3.28084</f>
+        <v>131.2336</v>
+      </c>
+      <c r="D2" s="9">
+        <f t="shared" ref="D2:D24" si="1">C2-4</f>
+        <v>127.2336</v>
+      </c>
+      <c r="F2">
+        <v>12.15</v>
+      </c>
+      <c r="G2" s="9">
+        <f t="shared" ref="G2:G24" si="2">F2*0.5+F2</f>
+        <v>18.225000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3">
+        <v>40</v>
+      </c>
+      <c r="C3" s="9">
+        <f t="shared" si="0"/>
+        <v>131.2336</v>
+      </c>
+      <c r="D3" s="9">
+        <f t="shared" si="1"/>
+        <v>127.2336</v>
+      </c>
+      <c r="F3">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="G3" s="9">
+        <f t="shared" si="2"/>
+        <v>25.650000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4">
+        <v>40</v>
+      </c>
+      <c r="C4" s="9">
+        <f t="shared" si="0"/>
+        <v>131.2336</v>
+      </c>
+      <c r="D4" s="9">
+        <f t="shared" si="1"/>
+        <v>127.2336</v>
+      </c>
+      <c r="F4">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="G4" s="9">
+        <f t="shared" si="2"/>
+        <v>25.650000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5">
+        <v>40</v>
+      </c>
+      <c r="C5" s="9">
+        <f t="shared" si="0"/>
+        <v>131.2336</v>
+      </c>
+      <c r="D5" s="9">
+        <f t="shared" si="1"/>
+        <v>127.2336</v>
+      </c>
+      <c r="F5">
+        <v>24.2</v>
+      </c>
+      <c r="G5" s="9">
+        <f t="shared" si="2"/>
+        <v>36.299999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6">
+        <v>40</v>
+      </c>
+      <c r="C6" s="9">
+        <f t="shared" si="0"/>
+        <v>131.2336</v>
+      </c>
+      <c r="D6" s="9">
+        <f t="shared" si="1"/>
+        <v>127.2336</v>
+      </c>
+      <c r="F6">
+        <v>24.2</v>
+      </c>
+      <c r="G6" s="9">
+        <f t="shared" si="2"/>
+        <v>36.299999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7">
+        <v>40</v>
+      </c>
+      <c r="C7" s="9">
+        <f t="shared" si="0"/>
+        <v>131.2336</v>
+      </c>
+      <c r="D7" s="9">
+        <f t="shared" si="1"/>
+        <v>127.2336</v>
+      </c>
+      <c r="F7">
+        <v>24.2</v>
+      </c>
+      <c r="G7" s="9">
+        <f t="shared" si="2"/>
+        <v>36.299999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8">
+        <v>40</v>
+      </c>
+      <c r="C8" s="9">
+        <f t="shared" si="0"/>
+        <v>131.2336</v>
+      </c>
+      <c r="D8" s="9">
+        <f t="shared" si="1"/>
+        <v>127.2336</v>
+      </c>
+      <c r="F8">
+        <v>24.2</v>
+      </c>
+      <c r="G8" s="9">
+        <f t="shared" si="2"/>
+        <v>36.299999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9">
+        <v>40</v>
+      </c>
+      <c r="C9" s="9">
+        <f t="shared" si="0"/>
+        <v>131.2336</v>
+      </c>
+      <c r="D9" s="9">
+        <f t="shared" si="1"/>
+        <v>127.2336</v>
+      </c>
+      <c r="F9">
+        <v>24.2</v>
+      </c>
+      <c r="G9" s="9">
+        <f t="shared" si="2"/>
+        <v>36.299999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10">
+        <v>40</v>
+      </c>
+      <c r="C10" s="9">
+        <f t="shared" si="0"/>
+        <v>131.2336</v>
+      </c>
+      <c r="D10" s="9">
+        <f t="shared" si="1"/>
+        <v>127.2336</v>
+      </c>
+      <c r="F10">
+        <v>24.2</v>
+      </c>
+      <c r="G10" s="9">
+        <f t="shared" si="2"/>
+        <v>36.299999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11">
+        <v>40</v>
+      </c>
+      <c r="C11" s="9">
+        <f t="shared" si="0"/>
+        <v>131.2336</v>
+      </c>
+      <c r="D11" s="9">
+        <f t="shared" si="1"/>
+        <v>127.2336</v>
+      </c>
+      <c r="F11">
+        <v>24.2</v>
+      </c>
+      <c r="G11" s="9">
+        <f t="shared" si="2"/>
+        <v>36.299999999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12">
+        <v>40</v>
+      </c>
+      <c r="C12" s="9">
+        <f t="shared" si="0"/>
+        <v>131.2336</v>
+      </c>
+      <c r="D12" s="9">
+        <f t="shared" si="1"/>
+        <v>127.2336</v>
+      </c>
+      <c r="F12">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="G12" s="9">
+        <f t="shared" si="2"/>
+        <v>49.050000000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13">
+        <v>40</v>
+      </c>
+      <c r="C13" s="9">
+        <f t="shared" si="0"/>
+        <v>131.2336</v>
+      </c>
+      <c r="D13" s="9">
+        <f t="shared" si="1"/>
+        <v>127.2336</v>
+      </c>
+      <c r="F13">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="G13" s="9">
+        <f t="shared" si="2"/>
+        <v>49.050000000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14" s="9">
+        <f t="shared" si="0"/>
+        <v>16.404199999999999</v>
+      </c>
+      <c r="D14" s="9">
+        <f t="shared" si="1"/>
+        <v>12.404199999999999</v>
+      </c>
+      <c r="F14">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="G14" s="9">
+        <f t="shared" si="2"/>
+        <v>49.050000000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>95</v>
+      </c>
+      <c r="B15">
+        <v>2.5</v>
+      </c>
+      <c r="C15" s="9">
+        <f t="shared" si="0"/>
+        <v>8.2020999999999997</v>
+      </c>
+      <c r="D15" s="9">
+        <f t="shared" si="1"/>
+        <v>4.2020999999999997</v>
+      </c>
+      <c r="F15">
+        <v>43.9</v>
+      </c>
+      <c r="G15" s="9">
+        <f t="shared" si="2"/>
+        <v>65.849999999999994</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B16">
+        <v>2.5</v>
+      </c>
+      <c r="C16" s="9">
+        <f t="shared" si="0"/>
+        <v>8.2020999999999997</v>
+      </c>
+      <c r="D16" s="9">
+        <f t="shared" si="1"/>
+        <v>4.2020999999999997</v>
+      </c>
+      <c r="F16">
+        <v>43.9</v>
+      </c>
+      <c r="G16" s="9">
+        <f t="shared" si="2"/>
+        <v>65.849999999999994</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17">
+        <v>2.5</v>
+      </c>
+      <c r="C17" s="9">
+        <f t="shared" si="0"/>
+        <v>8.2020999999999997</v>
+      </c>
+      <c r="D17" s="9">
+        <f t="shared" si="1"/>
+        <v>4.2020999999999997</v>
+      </c>
+      <c r="F17">
+        <v>43.9</v>
+      </c>
+      <c r="G17" s="9">
+        <f t="shared" si="2"/>
+        <v>65.849999999999994</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B18">
+        <v>2.5</v>
+      </c>
+      <c r="C18" s="9">
+        <f t="shared" si="0"/>
+        <v>8.2020999999999997</v>
+      </c>
+      <c r="D18" s="9">
+        <f t="shared" si="1"/>
+        <v>4.2020999999999997</v>
+      </c>
+      <c r="F18">
+        <v>43.9</v>
+      </c>
+      <c r="G18" s="9">
+        <f t="shared" si="2"/>
+        <v>65.849999999999994</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>99</v>
+      </c>
+      <c r="B19">
+        <v>2.5</v>
+      </c>
+      <c r="C19" s="9">
+        <f t="shared" si="0"/>
+        <v>8.2020999999999997</v>
+      </c>
+      <c r="D19" s="9">
+        <f t="shared" si="1"/>
+        <v>4.2020999999999997</v>
+      </c>
+      <c r="F19">
+        <v>43.9</v>
+      </c>
+      <c r="G19" s="9">
+        <f t="shared" si="2"/>
+        <v>65.849999999999994</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>100</v>
+      </c>
+      <c r="B20">
+        <v>2.5</v>
+      </c>
+      <c r="C20" s="9">
+        <f t="shared" si="0"/>
+        <v>8.2020999999999997</v>
+      </c>
+      <c r="D20" s="9">
+        <f t="shared" si="1"/>
+        <v>4.2020999999999997</v>
+      </c>
+      <c r="F20">
+        <v>56.4</v>
+      </c>
+      <c r="G20" s="9">
+        <f t="shared" si="2"/>
+        <v>84.6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>101</v>
+      </c>
+      <c r="B21">
+        <v>2.5</v>
+      </c>
+      <c r="C21" s="9">
+        <f t="shared" si="0"/>
+        <v>8.2020999999999997</v>
+      </c>
+      <c r="D21" s="9">
+        <f t="shared" si="1"/>
+        <v>4.2020999999999997</v>
+      </c>
+      <c r="F21">
+        <v>56.4</v>
+      </c>
+      <c r="G21" s="9">
+        <f t="shared" si="2"/>
+        <v>84.6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>102</v>
+      </c>
+      <c r="B22">
+        <v>3.5</v>
+      </c>
+      <c r="C22" s="9">
+        <f t="shared" si="0"/>
+        <v>11.482939999999999</v>
+      </c>
+      <c r="D22" s="9">
+        <f t="shared" si="1"/>
+        <v>7.4829399999999993</v>
+      </c>
+      <c r="F22">
+        <v>45</v>
+      </c>
+      <c r="G22" s="9">
+        <f t="shared" si="2"/>
+        <v>67.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>103</v>
+      </c>
+      <c r="B23">
+        <v>3.5</v>
+      </c>
+      <c r="C23" s="9">
+        <f t="shared" si="0"/>
+        <v>11.482939999999999</v>
+      </c>
+      <c r="D23" s="9">
+        <f t="shared" si="1"/>
+        <v>7.4829399999999993</v>
+      </c>
+      <c r="F23">
+        <v>45</v>
+      </c>
+      <c r="G23" s="9">
+        <f t="shared" si="2"/>
+        <v>67.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>104</v>
+      </c>
+      <c r="B24">
+        <v>6</v>
+      </c>
+      <c r="C24" s="9">
+        <f t="shared" si="0"/>
+        <v>19.685040000000001</v>
+      </c>
+      <c r="D24" s="9">
+        <f t="shared" si="1"/>
+        <v>15.685040000000001</v>
+      </c>
+      <c r="F24">
+        <v>56.4</v>
+      </c>
+      <c r="G24" s="9">
+        <f t="shared" si="2"/>
+        <v>84.6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added new model without Infrastructure as well as some graphics
</commit_message>
<xml_diff>
--- a/ModelsData/gab_soils_dev2.xlsx
+++ b/ModelsData/gab_soils_dev2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9465" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9465" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="gab_soils_dev2" sheetId="1" r:id="rId1"/>
@@ -1211,7 +1211,7 @@
   <dimension ref="A1:S237"/>
   <sheetViews>
     <sheetView topLeftCell="A200" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1:S1048576"/>
+      <selection activeCell="W224" sqref="W224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15208,8 +15208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B44"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17259,7 +17259,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:A31"/>
     </sheetView>
   </sheetViews>
@@ -18111,8 +18111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>